<commit_message>
Update test data in statistic of soberity
</commit_message>
<xml_diff>
--- a/rzeczowniki/rzeczowniki.xlsx
+++ b/rzeczowniki/rzeczowniki.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\informa\Semestr 7\NarzedziaSztucznejIntligencji\cw\cw_5\rzeczowniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{50BA7DBC-EE48-4B1E-85FA-6A70785821FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB6F34A-5B2C-40A4-9CD0-19E65A357C29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="792" yWindow="312" windowWidth="17280" windowHeight="10692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rzeczowniki" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
   <si>
     <t>kacet</t>
   </si>
@@ -178,13 +178,7 @@
     <t>Dardyjka</t>
   </si>
   <si>
-    <t>darek</t>
-  </si>
-  <si>
     <t>Darek</t>
-  </si>
-  <si>
-    <t>dargijski</t>
   </si>
   <si>
     <t>Daria</t>
@@ -688,7 +682,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1540,11 +1534,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C222"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:C220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A200" workbookViewId="0">
-      <selection activeCell="F218" sqref="F218"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102:B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2350,41 +2344,26 @@
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B102">
-        <v>101</v>
-      </c>
       <c r="C102" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103">
-        <v>102</v>
-      </c>
       <c r="C103" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104">
-        <v>103</v>
-      </c>
       <c r="C104" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B105">
-        <v>104</v>
-      </c>
       <c r="C105" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B106">
-        <v>105</v>
-      </c>
       <c r="C106" t="s">
         <v>104</v>
       </c>
@@ -3031,7 +3010,7 @@
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B187">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C187" t="s">
         <v>185</v>
@@ -3039,7 +3018,7 @@
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B188">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C188" t="s">
         <v>186</v>
@@ -3047,7 +3026,7 @@
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B189">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C189" t="s">
         <v>187</v>
@@ -3055,7 +3034,7 @@
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B190">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C190" t="s">
         <v>188</v>
@@ -3063,7 +3042,7 @@
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B191">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C191" t="s">
         <v>189</v>
@@ -3071,7 +3050,7 @@
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B192">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C192" t="s">
         <v>190</v>
@@ -3079,7 +3058,7 @@
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B193">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C193" t="s">
         <v>191</v>
@@ -3087,7 +3066,7 @@
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B194">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C194" t="s">
         <v>192</v>
@@ -3095,7 +3074,7 @@
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B195">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C195" t="s">
         <v>193</v>
@@ -3103,7 +3082,7 @@
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B196">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C196" t="s">
         <v>194</v>
@@ -3111,7 +3090,7 @@
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B197">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C197" t="s">
         <v>195</v>
@@ -3119,7 +3098,7 @@
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B198">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C198" t="s">
         <v>196</v>
@@ -3127,7 +3106,7 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B199">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C199" t="s">
         <v>197</v>
@@ -3135,7 +3114,7 @@
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B200">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C200" t="s">
         <v>198</v>
@@ -3143,7 +3122,7 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B201">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C201" t="s">
         <v>199</v>
@@ -3151,7 +3130,7 @@
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B202">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C202" t="s">
         <v>200</v>
@@ -3159,7 +3138,7 @@
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B203">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C203" t="s">
         <v>201</v>
@@ -3167,7 +3146,7 @@
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B204">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C204" t="s">
         <v>202</v>
@@ -3175,7 +3154,7 @@
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B205">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C205" t="s">
         <v>203</v>
@@ -3183,7 +3162,7 @@
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B206">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C206" t="s">
         <v>204</v>
@@ -3191,7 +3170,7 @@
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B207">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C207" t="s">
         <v>205</v>
@@ -3199,7 +3178,7 @@
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B208">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C208" t="s">
         <v>206</v>
@@ -3207,7 +3186,7 @@
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B209">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C209" t="s">
         <v>207</v>
@@ -3215,7 +3194,7 @@
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B210">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C210" t="s">
         <v>208</v>
@@ -3223,7 +3202,7 @@
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B211">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C211" t="s">
         <v>209</v>
@@ -3231,7 +3210,7 @@
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B212">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C212" t="s">
         <v>210</v>
@@ -3239,7 +3218,7 @@
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B213">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C213" t="s">
         <v>211</v>
@@ -3247,7 +3226,7 @@
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B214">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C214" t="s">
         <v>212</v>
@@ -3255,7 +3234,7 @@
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B215">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C215" t="s">
         <v>213</v>
@@ -3263,7 +3242,7 @@
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B216">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C216" t="s">
         <v>214</v>
@@ -3271,7 +3250,7 @@
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B217">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C217" t="s">
         <v>215</v>
@@ -3279,7 +3258,7 @@
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B218">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C218" t="s">
         <v>216</v>
@@ -3287,7 +3266,7 @@
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B219">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C219" t="s">
         <v>217</v>
@@ -3295,26 +3274,10 @@
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B220">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C220" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B221">
-        <v>220</v>
-      </c>
-      <c r="C221" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B222">
-        <v>221</v>
-      </c>
-      <c r="C222" t="s">
-        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add csv transision files
</commit_message>
<xml_diff>
--- a/rzeczowniki/rzeczowniki.xlsx
+++ b/rzeczowniki/rzeczowniki.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\informa\Semestr 7\NarzedziaSztucznejIntligencji\cw\cw_5\rzeczowniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB6F34A-5B2C-40A4-9CD0-19E65A357C29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A0F33D-2BB0-4B32-972A-DC54FE5C00F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="792" yWindow="312" windowWidth="17280" windowHeight="10692" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="200">
   <si>
     <t>kacet</t>
   </si>
@@ -322,24 +322,6 @@
     <t>madrytka</t>
   </si>
   <si>
-    <t>madurski</t>
-  </si>
-  <si>
-    <t>Madzia</t>
-  </si>
-  <si>
-    <t>Madziar</t>
-  </si>
-  <si>
-    <t>madziaryzacja</t>
-  </si>
-  <si>
-    <t>madziaryzm</t>
-  </si>
-  <si>
-    <t>maestria</t>
-  </si>
-  <si>
     <t>maestro</t>
   </si>
   <si>
@@ -484,9 +466,6 @@
     <t>palatyn</t>
   </si>
   <si>
-    <t>Palatyn</t>
-  </si>
-  <si>
     <t>Palatynat</t>
   </si>
   <si>
@@ -586,9 +565,6 @@
     <t>wata</t>
   </si>
   <si>
-    <t>wata cukrowa</t>
-  </si>
-  <si>
     <t>wataga</t>
   </si>
   <si>
@@ -634,9 +610,6 @@
     <t>wawrzyn</t>
   </si>
   <si>
-    <t>Wawrzyn</t>
-  </si>
-  <si>
     <t>Wawrzyniec</t>
   </si>
   <si>
@@ -647,36 +620,6 @@
   </si>
   <si>
     <t>wazelina</t>
-  </si>
-  <si>
-    <t>wazon</t>
-  </si>
-  <si>
-    <t>wazonik</t>
-  </si>
-  <si>
-    <t>wbicie</t>
-  </si>
-  <si>
-    <t>wbieganie</t>
-  </si>
-  <si>
-    <t>wbijanie</t>
-  </si>
-  <si>
-    <t>wchodzenie</t>
-  </si>
-  <si>
-    <t>wcielanie</t>
-  </si>
-  <si>
-    <t>wcielenie</t>
-  </si>
-  <si>
-    <t>wcieranie</t>
-  </si>
-  <si>
-    <t>wcierka</t>
   </si>
 </sst>
 </file>
@@ -1535,10 +1478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C220"/>
+  <dimension ref="B2:C201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102:B106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" activeCellId="1" sqref="B206:D211 H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2344,26 +2287,41 @@
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>101</v>
+      </c>
       <c r="C102" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>102</v>
+      </c>
       <c r="C103" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>103</v>
+      </c>
       <c r="C104" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>104</v>
+      </c>
       <c r="C105" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>105</v>
+      </c>
       <c r="C106" t="s">
         <v>104</v>
       </c>
@@ -3010,7 +2968,7 @@
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B187">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C187" t="s">
         <v>185</v>
@@ -3018,7 +2976,7 @@
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B188">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C188" t="s">
         <v>186</v>
@@ -3026,7 +2984,7 @@
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B189">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C189" t="s">
         <v>187</v>
@@ -3034,7 +2992,7 @@
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B190">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C190" t="s">
         <v>188</v>
@@ -3042,7 +3000,7 @@
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B191">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C191" t="s">
         <v>189</v>
@@ -3050,7 +3008,7 @@
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B192">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C192" t="s">
         <v>190</v>
@@ -3058,7 +3016,7 @@
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B193">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C193" t="s">
         <v>191</v>
@@ -3066,7 +3024,7 @@
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B194">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C194" t="s">
         <v>192</v>
@@ -3074,7 +3032,7 @@
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B195">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C195" t="s">
         <v>193</v>
@@ -3082,7 +3040,7 @@
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B196">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C196" t="s">
         <v>194</v>
@@ -3090,7 +3048,7 @@
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B197">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C197" t="s">
         <v>195</v>
@@ -3098,7 +3056,7 @@
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B198">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C198" t="s">
         <v>196</v>
@@ -3106,7 +3064,7 @@
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B199">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C199" t="s">
         <v>197</v>
@@ -3114,7 +3072,7 @@
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B200">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C200" t="s">
         <v>198</v>
@@ -3122,162 +3080,10 @@
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B201">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C201" t="s">
         <v>199</v>
-      </c>
-    </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B202">
-        <v>202</v>
-      </c>
-      <c r="C202" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B203">
-        <v>203</v>
-      </c>
-      <c r="C203" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B204">
-        <v>204</v>
-      </c>
-      <c r="C204" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B205">
-        <v>205</v>
-      </c>
-      <c r="C205" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B206">
-        <v>206</v>
-      </c>
-      <c r="C206" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B207">
-        <v>207</v>
-      </c>
-      <c r="C207" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B208">
-        <v>208</v>
-      </c>
-      <c r="C208" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B209">
-        <v>209</v>
-      </c>
-      <c r="C209" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B210">
-        <v>210</v>
-      </c>
-      <c r="C210" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B211">
-        <v>211</v>
-      </c>
-      <c r="C211" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B212">
-        <v>212</v>
-      </c>
-      <c r="C212" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B213">
-        <v>213</v>
-      </c>
-      <c r="C213" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B214">
-        <v>214</v>
-      </c>
-      <c r="C214" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B215">
-        <v>215</v>
-      </c>
-      <c r="C215" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B216">
-        <v>216</v>
-      </c>
-      <c r="C216" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B217">
-        <v>218</v>
-      </c>
-      <c r="C217" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B218">
-        <v>219</v>
-      </c>
-      <c r="C218" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B219">
-        <v>220</v>
-      </c>
-      <c r="C219" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B220">
-        <v>221</v>
-      </c>
-      <c r="C220" t="s">
-        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>